<commit_message>
TensorFlow 설치 및 Test 가이드
</commit_message>
<xml_diff>
--- a/Blog/Python/Tutorial/pandas/foo.xlsx
+++ b/Blog/Python/Tutorial/pandas/foo.xlsx
@@ -426,7 +426,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.5992946145410919</v>
+        <v>0.007879177902933363</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -437,13 +437,13 @@
         <v>41276</v>
       </c>
       <c r="B3">
-        <v>-0.9015980506402503</v>
+        <v>-0.4027513658717083</v>
       </c>
       <c r="C3">
-        <v>-1.678150775823147</v>
+        <v>-0.4661884778718272</v>
       </c>
       <c r="D3">
-        <v>-0.999940904707314</v>
+        <v>0.431977463267512</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -457,13 +457,13 @@
         <v>41277</v>
       </c>
       <c r="B4">
-        <v>-0.5610127474310403</v>
+        <v>-0.7820964899011106</v>
       </c>
       <c r="C4">
-        <v>-2.697689034159498</v>
+        <v>-1.291112248493917</v>
       </c>
       <c r="D4">
-        <v>0.9344770630951094</v>
+        <v>-1.417005508671151</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -477,13 +477,13 @@
         <v>41278</v>
       </c>
       <c r="B5">
-        <v>-1.326012350554234</v>
+        <v>0.351073541901304</v>
       </c>
       <c r="C5">
-        <v>-0.3961016277249444</v>
+        <v>0.523717141809419</v>
       </c>
       <c r="D5">
-        <v>-1.688932166605141</v>
+        <v>2.287742462260006</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -497,13 +497,13 @@
         <v>41279</v>
       </c>
       <c r="B6">
-        <v>-0.1561873332458719</v>
+        <v>-0.8622086857614417</v>
       </c>
       <c r="C6">
-        <v>1.911771468776793</v>
+        <v>-0.4437661975110234</v>
       </c>
       <c r="D6">
-        <v>-0.7037718369216818</v>
+        <v>2.173105040264365</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -517,13 +517,13 @@
         <v>41280</v>
       </c>
       <c r="B7">
-        <v>0.4180456989618921</v>
+        <v>1.457248943882707</v>
       </c>
       <c r="C7">
-        <v>-0.7420946950008535</v>
+        <v>0.5567061355003813</v>
       </c>
       <c r="D7">
-        <v>1.127068615156783</v>
+        <v>0.7582402414817506</v>
       </c>
       <c r="E7">
         <v>5</v>

</xml_diff>